<commit_message>
aggiunto codice esempio PPO
- aggiornato gym da 0.9 a 0.21
- inserito codice funzionante esempio PPO
</commit_message>
<xml_diff>
--- a/Simulazioni_RL/Risultati/adult#001_clear.xlsx
+++ b/Simulazioni_RL/Risultati/adult#001_clear.xlsx
@@ -488,7 +488,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>44880.50035407714</v>
+        <v>44881.50060109999</v>
       </c>
       <c r="B2" t="n">
         <v>138.56</v>
@@ -517,7 +517,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>44880.50243741048</v>
+        <v>44881.50268443332</v>
       </c>
       <c r="B3" t="n">
         <v>138.5600000000011</v>
@@ -546,7 +546,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>44880.50452074381</v>
+        <v>44881.50476776665</v>
       </c>
       <c r="B4" t="n">
         <v>138.5599999998948</v>
@@ -575,7 +575,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>44880.50660407714</v>
+        <v>44881.50685109999</v>
       </c>
       <c r="B5" t="n">
         <v>138.5599999986664</v>
@@ -604,7 +604,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>44880.50868741047</v>
+        <v>44881.50893443332</v>
       </c>
       <c r="B6" t="n">
         <v>138.5599999927699</v>
@@ -633,7 +633,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>44880.51077074381</v>
+        <v>44881.51101776666</v>
       </c>
       <c r="B7" t="n">
         <v>138.5599999744941</v>
@@ -662,7 +662,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>44880.51285407714</v>
+        <v>44881.51310109999</v>
       </c>
       <c r="B8" t="n">
         <v>138.5599999308572</v>
@@ -691,7 +691,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>44880.51493741047</v>
+        <v>44881.51518443332</v>
       </c>
       <c r="B9" t="n">
         <v>138.5599998430926</v>
@@ -720,7 +720,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>44880.51702074381</v>
+        <v>44881.51726776666</v>
       </c>
       <c r="B10" t="n">
         <v>138.5599996866284</v>
@@ -749,7 +749,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>44880.51910407714</v>
+        <v>44881.51935109999</v>
       </c>
       <c r="B11" t="n">
         <v>138.5599994314249</v>
@@ -778,7 +778,7 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>44880.52118741047</v>
+        <v>44881.52143443332</v>
       </c>
       <c r="B12" t="n">
         <v>138.5599990425436</v>
@@ -807,7 +807,7 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>44880.5232707438</v>
+        <v>44881.52351776665</v>
       </c>
       <c r="B13" t="n">
         <v>138.5599984808477</v>
@@ -836,7 +836,7 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>44880.52535407714</v>
+        <v>44881.52560109999</v>
       </c>
       <c r="B14" t="n">
         <v>138.5599977037598</v>
@@ -865,7 +865,7 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>44880.52743741048</v>
+        <v>44881.52768443332</v>
       </c>
       <c r="B15" t="n">
         <v>138.5599966660216</v>
@@ -894,7 +894,7 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>44880.52952074381</v>
+        <v>44881.52976776665</v>
       </c>
       <c r="B16" t="n">
         <v>138.559995320426</v>
@@ -923,7 +923,7 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>44880.53160407714</v>
+        <v>44881.53185109999</v>
       </c>
       <c r="B17" t="n">
         <v>138.5599936184957</v>
@@ -952,7 +952,7 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>44880.53368741048</v>
+        <v>44881.53393443332</v>
       </c>
       <c r="B18" t="n">
         <v>138.5599915111018</v>
@@ -981,7 +981,7 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>44880.53577074381</v>
+        <v>44881.53601776665</v>
       </c>
       <c r="B19" t="n">
         <v>138.5599889490141</v>
@@ -1010,7 +1010,7 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>44880.53785407714</v>
+        <v>44881.53810109999</v>
       </c>
       <c r="B20" t="n">
         <v>138.559985883385</v>
@@ -1039,7 +1039,7 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>44880.53993741047</v>
+        <v>44881.54018443332</v>
       </c>
       <c r="B21" t="n">
         <v>138.5599822661682</v>
@@ -1068,7 +1068,7 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>44880.54202074381</v>
+        <v>44881.54226776666</v>
       </c>
       <c r="B22" t="n">
         <v>138.559978050476</v>
@@ -1097,7 +1097,7 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>44880.54410407714</v>
+        <v>44881.54435109999</v>
       </c>
       <c r="B23" t="n">
         <v>138.5599734796085</v>
@@ -1126,7 +1126,7 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>44880.54618741047</v>
+        <v>44881.54643443332</v>
       </c>
       <c r="B24" t="n">
         <v>138.5606811612882</v>
@@ -1155,7 +1155,7 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>44880.54827074381</v>
+        <v>44881.54851776666</v>
       </c>
       <c r="B25" t="n">
         <v>138.5758338091874</v>
@@ -1184,7 +1184,7 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>44880.55035407714</v>
+        <v>44881.55060109999</v>
       </c>
       <c r="B26" t="n">
         <v>138.6605464590204</v>
@@ -1213,7 +1213,7 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>44880.55243741047</v>
+        <v>44881.55268443332</v>
       </c>
       <c r="B27" t="n">
         <v>138.9213843923341</v>
@@ -1242,7 +1242,7 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>44880.5545207438</v>
+        <v>44881.55476776665</v>
       </c>
       <c r="B28" t="n">
         <v>139.5069157618104</v>
@@ -1271,7 +1271,7 @@
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>44880.55660407714</v>
+        <v>44881.55685109999</v>
       </c>
       <c r="B29" t="n">
         <v>140.5913836830076</v>
@@ -1300,7 +1300,7 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>44880.55868741048</v>
+        <v>44881.55893443332</v>
       </c>
       <c r="B30" t="n">
         <v>142.3565110859411</v>
@@ -1329,7 +1329,7 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>44880.56077074381</v>
+        <v>44881.56101776665</v>
       </c>
       <c r="B31" t="n">
         <v>144.953371963437</v>
@@ -1358,7 +1358,7 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>44880.56285407714</v>
+        <v>44881.56310109999</v>
       </c>
       <c r="B32" t="n">
         <v>148.4534273348439</v>
@@ -1387,7 +1387,7 @@
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>44880.56493741048</v>
+        <v>44881.56518443332</v>
       </c>
       <c r="B33" t="n">
         <v>152.8250901838406</v>
@@ -1416,7 +1416,7 @@
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>44880.56702074381</v>
+        <v>44881.56726776665</v>
       </c>
       <c r="B34" t="n">
         <v>157.9326478834673</v>
@@ -1445,7 +1445,7 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>44880.56910407714</v>
+        <v>44881.56935109999</v>
       </c>
       <c r="B35" t="n">
         <v>163.5577599030571</v>
@@ -1474,7 +1474,7 @@
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>44880.57118741047</v>
+        <v>44881.57143443332</v>
       </c>
       <c r="B36" t="n">
         <v>169.4434344722648</v>
@@ -1503,7 +1503,7 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>44880.57327074381</v>
+        <v>44881.57351776666</v>
       </c>
       <c r="B37" t="n">
         <v>175.341417560203</v>
@@ -1532,7 +1532,7 @@
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>44880.57535407714</v>
+        <v>44881.57560109999</v>
       </c>
       <c r="B38" t="n">
         <v>181.0437050409912</v>
@@ -1561,7 +1561,7 @@
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>44880.57743741047</v>
+        <v>44881.57768443332</v>
       </c>
       <c r="B39" t="n">
         <v>186.3951912195193</v>
@@ -1590,7 +1590,7 @@
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>44880.57952074381</v>
+        <v>44881.57976776666</v>
       </c>
       <c r="B40" t="n">
         <v>191.2928204493224</v>
@@ -1619,7 +1619,7 @@
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>44880.58160407714</v>
+        <v>44881.58185109999</v>
       </c>
       <c r="B41" t="n">
         <v>195.6779151233904</v>
@@ -1648,7 +1648,7 @@
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>44880.58368741047</v>
+        <v>44881.58393443332</v>
       </c>
       <c r="B42" t="n">
         <v>199.526358868968</v>
@@ -1677,7 +1677,7 @@
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>44880.5857707438</v>
+        <v>44881.58601776665</v>
       </c>
       <c r="B43" t="n">
         <v>202.8391549367546</v>
@@ -1706,7 +1706,7 @@
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>44880.58785407714</v>
+        <v>44881.58810109999</v>
       </c>
       <c r="B44" t="n">
         <v>205.6344288521939</v>
@@ -1735,7 +1735,7 @@
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>44880.58993741048</v>
+        <v>44881.59018443332</v>
       </c>
       <c r="B45" t="n">
         <v>207.9411432007708</v>
@@ -1764,7 +1764,7 @@
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>44880.59202074381</v>
+        <v>44881.59226776665</v>
       </c>
       <c r="B46" t="n">
         <v>209.7944116233752</v>
@@ -1793,7 +1793,7 @@
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>44880.59410407714</v>
+        <v>44881.59435109999</v>
       </c>
       <c r="B47" t="n">
         <v>211.2321533354801</v>
@@ -1822,7 +1822,7 @@
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>44880.59618741048</v>
+        <v>44881.59643443332</v>
       </c>
       <c r="B48" t="n">
         <v>212.2928022449778</v>
@@ -1851,7 +1851,7 @@
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>44880.59827074381</v>
+        <v>44881.59851776665</v>
       </c>
       <c r="B49" t="n">
         <v>213.0138104131109</v>
@@ -1880,7 +1880,7 @@
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
-        <v>44880.60035407714</v>
+        <v>44881.60060109999</v>
       </c>
       <c r="B50" t="n">
         <v>213.4307298855713</v>
@@ -1909,7 +1909,7 @@
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
-        <v>44880.60243741047</v>
+        <v>44881.60268443332</v>
       </c>
       <c r="B51" t="n">
         <v>213.5767032445664</v>
@@ -1938,7 +1938,7 @@
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
-        <v>44880.60452074381</v>
+        <v>44881.60476776666</v>
       </c>
       <c r="B52" t="n">
         <v>213.482234510414</v>
@@ -1967,7 +1967,7 @@
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
-        <v>44880.60660407714</v>
+        <v>44881.60685109999</v>
       </c>
       <c r="B53" t="n">
         <v>213.1751459730963</v>
@@ -1996,7 +1996,7 @@
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
-        <v>44880.60868741047</v>
+        <v>44881.60893443332</v>
       </c>
       <c r="B54" t="n">
         <v>212.6806531424355</v>
@@ -2025,7 +2025,7 @@
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
-        <v>44880.61077074381</v>
+        <v>44881.61101776666</v>
       </c>
       <c r="B55" t="n">
         <v>212.0215101838714</v>
@@ -2054,7 +2054,7 @@
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
-        <v>44880.61285407714</v>
+        <v>44881.61310109999</v>
       </c>
       <c r="B56" t="n">
         <v>211.2181931378731</v>
@@ -2083,7 +2083,7 @@
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
-        <v>44880.61493741047</v>
+        <v>44881.61518443332</v>
       </c>
       <c r="B57" t="n">
         <v>210.2890990511079</v>
@@ -2112,7 +2112,7 @@
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
-        <v>44880.6170207438</v>
+        <v>44881.61726776665</v>
       </c>
       <c r="B58" t="n">
         <v>209.2507468657183</v>
@@ -2141,7 +2141,7 @@
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
-        <v>44880.61910407714</v>
+        <v>44881.61935109999</v>
       </c>
       <c r="B59" t="n">
         <v>208.1179713210128</v>
@@ -2170,7 +2170,7 @@
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
-        <v>44880.62118741048</v>
+        <v>44881.62143443332</v>
       </c>
       <c r="B60" t="n">
         <v>206.9041048443084</v>
@@ -2199,7 +2199,7 @@
     </row>
     <row r="61">
       <c r="A61" s="2" t="n">
-        <v>44880.62327074381</v>
+        <v>44881.62351776665</v>
       </c>
       <c r="B61" t="n">
         <v>205.6211449187058</v>
@@ -2228,7 +2228,7 @@
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
-        <v>44880.62535407714</v>
+        <v>44881.62560109999</v>
       </c>
       <c r="B62" t="n">
         <v>204.2799060680334</v>
@@ -2257,7 +2257,7 @@
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
-        <v>44880.62743741048</v>
+        <v>44881.62768443332</v>
       </c>
       <c r="B63" t="n">
         <v>202.8901566517287</v>
@@ -2286,7 +2286,7 @@
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
-        <v>44880.62952074381</v>
+        <v>44881.62976776665</v>
       </c>
       <c r="B64" t="n">
         <v>201.4607413022461</v>
@@ -2315,7 +2315,7 @@
     </row>
     <row r="65">
       <c r="A65" s="2" t="n">
-        <v>44880.63160407714</v>
+        <v>44881.63185109999</v>
       </c>
       <c r="B65" t="n">
         <v>199.9996901988851</v>
@@ -2344,7 +2344,7 @@
     </row>
     <row r="66">
       <c r="A66" s="2" t="n">
-        <v>44880.63368741047</v>
+        <v>44881.63393443332</v>
       </c>
       <c r="B66" t="n">
         <v>198.5143165499267</v>
@@ -2373,7 +2373,7 @@
     </row>
     <row r="67">
       <c r="A67" s="2" t="n">
-        <v>44880.63577074381</v>
+        <v>44881.63601776666</v>
       </c>
       <c r="B67" t="n">
         <v>197.0113037167519</v>
@@ -2402,7 +2402,7 @@
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
-        <v>44880.63785407714</v>
+        <v>44881.63810109999</v>
       </c>
       <c r="B68" t="n">
         <v>195.4967834061341</v>
@@ -2431,7 +2431,7 @@
     </row>
     <row r="69">
       <c r="A69" s="2" t="n">
-        <v>44880.63993741047</v>
+        <v>44881.64018443332</v>
       </c>
       <c r="B69" t="n">
         <v>193.9764063129518</v>
@@ -2460,7 +2460,7 @@
     </row>
     <row r="70">
       <c r="A70" s="2" t="n">
-        <v>44880.64202074381</v>
+        <v>44881.64226776666</v>
       </c>
       <c r="B70" t="n">
         <v>192.4554065381906</v>
@@ -2489,7 +2489,7 @@
     </row>
     <row r="71">
       <c r="A71" s="2" t="n">
-        <v>44880.64410407714</v>
+        <v>44881.64435109999</v>
       </c>
       <c r="B71" t="n">
         <v>190.9386610528188</v>
@@ -2518,7 +2518,7 @@
     </row>
     <row r="72">
       <c r="A72" s="2" t="n">
-        <v>44880.64618741047</v>
+        <v>44881.64643443332</v>
       </c>
       <c r="B72" t="n">
         <v>189.4307454393996</v>
@@ -2547,7 +2547,7 @@
     </row>
     <row r="73">
       <c r="A73" s="2" t="n">
-        <v>44880.6482707438</v>
+        <v>44881.64851776665</v>
       </c>
       <c r="B73" t="n">
         <v>187.9359871304925</v>
@@ -2576,7 +2576,7 @@
     </row>
     <row r="74">
       <c r="A74" s="2" t="n">
-        <v>44880.65035407714</v>
+        <v>44881.65060109999</v>
       </c>
       <c r="B74" t="n">
         <v>186.4585173857465</v>
@@ -2605,7 +2605,7 @@
     </row>
     <row r="75">
       <c r="A75" s="2" t="n">
-        <v>44880.65243741048</v>
+        <v>44881.65268443332</v>
       </c>
       <c r="B75" t="n">
         <v>185.002323318719</v>
@@ -2634,7 +2634,7 @@
     </row>
     <row r="76">
       <c r="A76" s="2" t="n">
-        <v>44880.65452074381</v>
+        <v>44881.65476776665</v>
       </c>
       <c r="B76" t="n">
         <v>183.5713014127506</v>
@@ -2663,7 +2663,7 @@
     </row>
     <row r="77">
       <c r="A77" s="2" t="n">
-        <v>44880.65660407714</v>
+        <v>44881.65685109999</v>
       </c>
       <c r="B77" t="n">
         <v>182.1692820712786</v>
@@ -2692,7 +2692,7 @@
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
-        <v>44880.65868741048</v>
+        <v>44881.65893443332</v>
       </c>
       <c r="B78" t="n">
         <v>180.7999379120656</v>
@@ -2721,7 +2721,7 @@
     </row>
     <row r="79">
       <c r="A79" s="2" t="n">
-        <v>44880.66077074381</v>
+        <v>44881.66101776665</v>
       </c>
       <c r="B79" t="n">
         <v>179.4822171304289</v>
@@ -2750,7 +2750,7 @@
     </row>
     <row r="80">
       <c r="A80" s="2" t="n">
-        <v>44880.66285407714</v>
+        <v>44881.66310109999</v>
       </c>
       <c r="B80" t="n">
         <v>178.4839860450501</v>
@@ -2779,7 +2779,7 @@
     </row>
     <row r="81">
       <c r="A81" s="2" t="n">
-        <v>44880.66493741047</v>
+        <v>44881.66518443332</v>
       </c>
       <c r="B81" t="n">
         <v>178.2116885846853</v>
@@ -2808,7 +2808,7 @@
     </row>
     <row r="82">
       <c r="A82" s="2" t="n">
-        <v>44880.66702074381</v>
+        <v>44881.66726776666</v>
       </c>
       <c r="B82" t="n">
         <v>178.7758482645653</v>
@@ -2837,7 +2837,7 @@
     </row>
     <row r="83">
       <c r="A83" s="2" t="n">
-        <v>44880.66910407714</v>
+        <v>44881.66935109999</v>
       </c>
       <c r="B83" t="n">
         <v>180.0514351016218</v>
@@ -2866,7 +2866,7 @@
     </row>
     <row r="84">
       <c r="A84" s="2" t="n">
-        <v>44880.67118741047</v>
+        <v>44881.67143443332</v>
       </c>
       <c r="B84" t="n">
         <v>181.7944394676312</v>
@@ -2895,7 +2895,7 @@
     </row>
     <row r="85">
       <c r="A85" s="2" t="n">
-        <v>44880.67327074381</v>
+        <v>44881.67351776666</v>
       </c>
       <c r="B85" t="n">
         <v>183.7412763872546</v>
@@ -2924,7 +2924,7 @@
     </row>
     <row r="86">
       <c r="A86" s="2" t="n">
-        <v>44880.67535407714</v>
+        <v>44881.67560109999</v>
       </c>
       <c r="B86" t="n">
         <v>185.6697358658026</v>
@@ -2953,7 +2953,7 @@
     </row>
     <row r="87">
       <c r="A87" s="2" t="n">
-        <v>44880.67743741047</v>
+        <v>44881.67768443332</v>
       </c>
       <c r="B87" t="n">
         <v>187.4195266421568</v>
@@ -2982,7 +2982,7 @@
     </row>
     <row r="88">
       <c r="A88" s="2" t="n">
-        <v>44880.6795207438</v>
+        <v>44881.67976776665</v>
       </c>
       <c r="B88" t="n">
         <v>188.8893523885694</v>
@@ -3011,7 +3011,7 @@
     </row>
     <row r="89">
       <c r="A89" s="2" t="n">
-        <v>44880.68160407714</v>
+        <v>44881.68185109999</v>
       </c>
       <c r="B89" t="n">
         <v>190.0252116248384</v>
@@ -3040,7 +3040,7 @@
     </row>
     <row r="90">
       <c r="A90" s="2" t="n">
-        <v>44880.68368741048</v>
+        <v>44881.68393443332</v>
       </c>
       <c r="B90" t="n">
         <v>190.8074936707712</v>
@@ -3069,7 +3069,7 @@
     </row>
     <row r="91">
       <c r="A91" s="2" t="n">
-        <v>44880.68577074381</v>
+        <v>44881.68601776665</v>
       </c>
       <c r="B91" t="n">
         <v>191.2398290098539</v>
@@ -3098,7 +3098,7 @@
     </row>
     <row r="92">
       <c r="A92" s="2" t="n">
-        <v>44880.68785407714</v>
+        <v>44881.68810109999</v>
       </c>
       <c r="B92" t="n">
         <v>191.3404472119197</v>
@@ -3127,7 +3127,7 @@
     </row>
     <row r="93">
       <c r="A93" s="2" t="n">
-        <v>44880.68993741048</v>
+        <v>44881.69018443332</v>
       </c>
       <c r="B93" t="n">
         <v>191.1358996246695</v>
@@ -3156,7 +3156,7 @@
     </row>
     <row r="94">
       <c r="A94" s="2" t="n">
-        <v>44880.69202074381</v>
+        <v>44881.69226776665</v>
       </c>
       <c r="B94" t="n">
         <v>190.6567151396728</v>
@@ -3185,7 +3185,7 @@
     </row>
     <row r="95">
       <c r="A95" s="2" t="n">
-        <v>44880.69410407714</v>
+        <v>44881.69435109999</v>
       </c>
       <c r="B95" t="n">
         <v>189.934524240508</v>
@@ -3214,7 +3214,7 @@
     </row>
     <row r="96">
       <c r="A96" s="2" t="n">
-        <v>44880.69618741047</v>
+        <v>44881.69643443332</v>
       </c>
       <c r="B96" t="n">
         <v>189.0002474406641</v>
@@ -3243,7 +3243,7 @@
     </row>
     <row r="97">
       <c r="A97" s="2" t="n">
-        <v>44880.69827074381</v>
+        <v>44881.69851776666</v>
       </c>
       <c r="B97" t="n">
         <v>187.8830287097096</v>
@@ -3272,7 +3272,7 @@
     </row>
     <row r="98">
       <c r="A98" s="2" t="n">
-        <v>44880.70035407714</v>
+        <v>44881.70060109999</v>
       </c>
       <c r="B98" t="n">
         <v>186.6096744444968</v>
@@ -3301,7 +3301,7 @@
     </row>
     <row r="99">
       <c r="A99" s="2" t="n">
-        <v>44880.70243741047</v>
+        <v>44881.70268443332</v>
       </c>
       <c r="B99" t="n">
         <v>185.204424748465</v>
@@ -3330,7 +3330,7 @@
     </row>
     <row r="100">
       <c r="A100" s="2" t="n">
-        <v>44880.70452074381</v>
+        <v>44881.70476776666</v>
       </c>
       <c r="B100" t="n">
         <v>183.6889329721793</v>
@@ -3359,7 +3359,7 @@
     </row>
     <row r="101">
       <c r="A101" s="2" t="n">
-        <v>44880.70660407714</v>
+        <v>44881.70685109999</v>
       </c>
       <c r="B101" t="n">
         <v>182.0822422365885</v>
@@ -3388,7 +3388,7 @@
     </row>
     <row r="102">
       <c r="A102" s="2" t="n">
-        <v>44880.70868741047</v>
+        <v>44881.70893443332</v>
       </c>
       <c r="B102" t="n">
         <v>180.4008097349049</v>
@@ -3417,7 +3417,7 @@
     </row>
     <row r="103">
       <c r="A103" s="2" t="n">
-        <v>44880.7107707438</v>
+        <v>44881.71101776665</v>
       </c>
       <c r="B103" t="n">
         <v>178.6590636911429</v>
@@ -3446,7 +3446,7 @@
     </row>
     <row r="104">
       <c r="A104" s="2" t="n">
-        <v>44880.71285407714</v>
+        <v>44881.71310109999</v>
       </c>
       <c r="B104" t="n">
         <v>176.8696886194843</v>
@@ -3475,7 +3475,7 @@
     </row>
     <row r="105">
       <c r="A105" s="2" t="n">
-        <v>44880.71493741048</v>
+        <v>44881.71518443332</v>
       </c>
       <c r="B105" t="n">
         <v>175.0438008299371</v>
@@ -3504,7 +3504,7 @@
     </row>
     <row r="106">
       <c r="A106" s="2" t="n">
-        <v>44880.71702074381</v>
+        <v>44881.71726776665</v>
       </c>
       <c r="B106" t="n">
         <v>173.1911237361004</v>
@@ -3533,7 +3533,7 @@
     </row>
     <row r="107">
       <c r="A107" s="2" t="n">
-        <v>44880.71910407714</v>
+        <v>44881.71935109999</v>
       </c>
       <c r="B107" t="n">
         <v>171.3201546577692</v>
@@ -3562,7 +3562,7 @@
     </row>
     <row r="108">
       <c r="A108" s="2" t="n">
-        <v>44880.72118741048</v>
+        <v>44881.72143443332</v>
       </c>
       <c r="B108" t="n">
         <v>169.4754007311149</v>
@@ -3591,7 +3591,7 @@
     </row>
     <row r="109">
       <c r="A109" s="2" t="n">
-        <v>44880.72327074381</v>
+        <v>44881.72351776665</v>
       </c>
       <c r="B109" t="n">
         <v>167.9109462790697</v>
@@ -3620,7 +3620,7 @@
     </row>
     <row r="110">
       <c r="A110" s="2" t="n">
-        <v>44880.72535407714</v>
+        <v>44881.72560109999</v>
       </c>
       <c r="B110" t="n">
         <v>166.8699132621484</v>
@@ -3649,7 +3649,7 @@
     </row>
     <row r="111">
       <c r="A111" s="2" t="n">
-        <v>44880.72743741047</v>
+        <v>44881.72768443332</v>
       </c>
       <c r="B111" t="n">
         <v>166.4622377596964</v>
@@ -3678,7 +3678,7 @@
     </row>
     <row r="112">
       <c r="A112" s="2" t="n">
-        <v>44880.72952074381</v>
+        <v>44881.72976776666</v>
       </c>
       <c r="B112" t="n">
         <v>166.7463068947553</v>
@@ -3707,7 +3707,7 @@
     </row>
     <row r="113">
       <c r="A113" s="2" t="n">
-        <v>44880.73160407714</v>
+        <v>44881.73185109999</v>
       </c>
       <c r="B113" t="n">
         <v>167.7722512678529</v>
@@ -3736,7 +3736,7 @@
     </row>
     <row r="114">
       <c r="A114" s="2" t="n">
-        <v>44880.73368741047</v>
+        <v>44881.73393443332</v>
       </c>
       <c r="B114" t="n">
         <v>169.5892184828768</v>
@@ -3765,7 +3765,7 @@
     </row>
     <row r="115">
       <c r="A115" s="2" t="n">
-        <v>44880.73577074381</v>
+        <v>44881.73601776666</v>
       </c>
       <c r="B115" t="n">
         <v>172.1916501642761</v>
@@ -3794,7 +3794,7 @@
     </row>
     <row r="116">
       <c r="A116" s="2" t="n">
-        <v>44880.73785407714</v>
+        <v>44881.73810109999</v>
       </c>
       <c r="B116" t="n">
         <v>175.4810192208173</v>
@@ -3823,7 +3823,7 @@
     </row>
     <row r="117">
       <c r="A117" s="2" t="n">
-        <v>44880.73993741047</v>
+        <v>44881.74018443332</v>
       </c>
       <c r="B117" t="n">
         <v>179.2735499924243</v>
@@ -3852,7 +3852,7 @@
     </row>
     <row r="118">
       <c r="A118" s="2" t="n">
-        <v>44880.7420207438</v>
+        <v>44881.74226776665</v>
       </c>
       <c r="B118" t="n">
         <v>183.3361284704601</v>
@@ -3881,7 +3881,7 @@
     </row>
     <row r="119">
       <c r="A119" s="2" t="n">
-        <v>44880.74410407714</v>
+        <v>44881.74435109999</v>
       </c>
       <c r="B119" t="n">
         <v>187.4316183747051</v>
@@ -3910,7 +3910,7 @@
     </row>
     <row r="120">
       <c r="A120" s="2" t="n">
-        <v>44880.74618741048</v>
+        <v>44881.74643443332</v>
       </c>
       <c r="B120" t="n">
         <v>191.3535905976206</v>
@@ -3939,7 +3939,7 @@
     </row>
     <row r="121">
       <c r="A121" s="2" t="n">
-        <v>44880.74827074381</v>
+        <v>44881.74851776665</v>
       </c>
       <c r="B121" t="n">
         <v>194.9432319349993</v>
@@ -3968,7 +3968,7 @@
     </row>
     <row r="122">
       <c r="A122" s="2" t="n">
-        <v>44880.75035407714</v>
+        <v>44881.75060109999</v>
       </c>
       <c r="B122" t="n">
         <v>198.0918901444067</v>

</xml_diff>

<commit_message>
problema controller risolto in parte
- problema nel prendere CGM da parte dei due controller, per ora modificato in modo che prenda CGM ma non ancora dCGM
</commit_message>
<xml_diff>
--- a/Simulazioni_RL/Risultati/adult#001_clear.xlsx
+++ b/Simulazioni_RL/Risultati/adult#001_clear.xlsx
@@ -488,7 +488,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>44881.50060109999</v>
+        <v>44937.5003107185</v>
       </c>
       <c r="B2" t="n">
         <v>138.56</v>
@@ -517,7 +517,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>44881.50268443332</v>
+        <v>44937.50239405183</v>
       </c>
       <c r="B3" t="n">
         <v>138.5600000000011</v>
@@ -546,7 +546,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>44881.50476776665</v>
+        <v>44937.50447738516</v>
       </c>
       <c r="B4" t="n">
         <v>138.5599999998948</v>
@@ -575,7 +575,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>44881.50685109999</v>
+        <v>44937.5065607185</v>
       </c>
       <c r="B5" t="n">
         <v>138.5599999986664</v>
@@ -604,7 +604,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>44881.50893443332</v>
+        <v>44937.50864405183</v>
       </c>
       <c r="B6" t="n">
         <v>138.5599999927699</v>
@@ -633,7 +633,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>44881.51101776666</v>
+        <v>44937.51072738516</v>
       </c>
       <c r="B7" t="n">
         <v>138.5599999744941</v>
@@ -662,7 +662,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>44881.51310109999</v>
+        <v>44937.51281071849</v>
       </c>
       <c r="B8" t="n">
         <v>138.5599999308572</v>
@@ -691,7 +691,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>44881.51518443332</v>
+        <v>44937.51489405183</v>
       </c>
       <c r="B9" t="n">
         <v>138.5599998430926</v>
@@ -720,7 +720,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>44881.51726776666</v>
+        <v>44937.51697738516</v>
       </c>
       <c r="B10" t="n">
         <v>138.5599996866284</v>
@@ -749,7 +749,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>44881.51935109999</v>
+        <v>44937.51906071849</v>
       </c>
       <c r="B11" t="n">
         <v>138.5599994314249</v>
@@ -778,7 +778,7 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>44881.52143443332</v>
+        <v>44937.52114405183</v>
       </c>
       <c r="B12" t="n">
         <v>138.5599990425436</v>
@@ -807,7 +807,7 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>44881.52351776665</v>
+        <v>44937.52322738517</v>
       </c>
       <c r="B13" t="n">
         <v>138.5599984808477</v>
@@ -836,7 +836,7 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>44881.52560109999</v>
+        <v>44937.5253107185</v>
       </c>
       <c r="B14" t="n">
         <v>138.5599977037598</v>
@@ -865,7 +865,7 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>44881.52768443332</v>
+        <v>44937.52739405183</v>
       </c>
       <c r="B15" t="n">
         <v>138.5599966660216</v>
@@ -894,7 +894,7 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>44881.52976776665</v>
+        <v>44937.52947738516</v>
       </c>
       <c r="B16" t="n">
         <v>138.559995320426</v>
@@ -923,7 +923,7 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>44881.53185109999</v>
+        <v>44937.5315607185</v>
       </c>
       <c r="B17" t="n">
         <v>138.5599936184957</v>
@@ -952,7 +952,7 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>44881.53393443332</v>
+        <v>44937.53364405183</v>
       </c>
       <c r="B18" t="n">
         <v>138.5599915111018</v>
@@ -981,7 +981,7 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>44881.53601776665</v>
+        <v>44937.53572738516</v>
       </c>
       <c r="B19" t="n">
         <v>138.5599889490141</v>
@@ -1010,7 +1010,7 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>44881.53810109999</v>
+        <v>44937.5378107185</v>
       </c>
       <c r="B20" t="n">
         <v>138.559985883385</v>
@@ -1039,7 +1039,7 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>44881.54018443332</v>
+        <v>44937.53989405183</v>
       </c>
       <c r="B21" t="n">
         <v>138.5599822661682</v>
@@ -1068,7 +1068,7 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>44881.54226776666</v>
+        <v>44937.54197738516</v>
       </c>
       <c r="B22" t="n">
         <v>138.559978050476</v>
@@ -1097,7 +1097,7 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>44881.54435109999</v>
+        <v>44937.54406071849</v>
       </c>
       <c r="B23" t="n">
         <v>138.5599734796085</v>
@@ -1126,7 +1126,7 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>44881.54643443332</v>
+        <v>44937.54614405183</v>
       </c>
       <c r="B24" t="n">
         <v>138.5606811612882</v>
@@ -1155,7 +1155,7 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>44881.54851776666</v>
+        <v>44937.54822738516</v>
       </c>
       <c r="B25" t="n">
         <v>138.5758338091874</v>
@@ -1184,7 +1184,7 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>44881.55060109999</v>
+        <v>44937.55031071849</v>
       </c>
       <c r="B26" t="n">
         <v>138.6605464590204</v>
@@ -1213,7 +1213,7 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>44881.55268443332</v>
+        <v>44937.55239405183</v>
       </c>
       <c r="B27" t="n">
         <v>138.9213843923341</v>
@@ -1242,7 +1242,7 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>44881.55476776665</v>
+        <v>44937.55447738517</v>
       </c>
       <c r="B28" t="n">
         <v>139.5069157618104</v>
@@ -1271,7 +1271,7 @@
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>44881.55685109999</v>
+        <v>44937.5565607185</v>
       </c>
       <c r="B29" t="n">
         <v>140.5913836830076</v>
@@ -1300,7 +1300,7 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>44881.55893443332</v>
+        <v>44937.55864405183</v>
       </c>
       <c r="B30" t="n">
         <v>142.3565110859411</v>
@@ -1329,7 +1329,7 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>44881.56101776665</v>
+        <v>44937.56072738516</v>
       </c>
       <c r="B31" t="n">
         <v>144.953371963437</v>
@@ -1358,7 +1358,7 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>44881.56310109999</v>
+        <v>44937.5628107185</v>
       </c>
       <c r="B32" t="n">
         <v>148.4534273348439</v>
@@ -1387,7 +1387,7 @@
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>44881.56518443332</v>
+        <v>44937.56489405183</v>
       </c>
       <c r="B33" t="n">
         <v>152.8250901838406</v>
@@ -1416,7 +1416,7 @@
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>44881.56726776665</v>
+        <v>44937.56697738516</v>
       </c>
       <c r="B34" t="n">
         <v>157.9326478834673</v>
@@ -1445,7 +1445,7 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>44881.56935109999</v>
+        <v>44937.5690607185</v>
       </c>
       <c r="B35" t="n">
         <v>163.5577599030571</v>
@@ -1474,7 +1474,7 @@
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>44881.57143443332</v>
+        <v>44937.57114405183</v>
       </c>
       <c r="B36" t="n">
         <v>169.4434344722648</v>
@@ -1503,7 +1503,7 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>44881.57351776666</v>
+        <v>44937.57322738516</v>
       </c>
       <c r="B37" t="n">
         <v>175.341417560203</v>
@@ -1532,7 +1532,7 @@
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>44881.57560109999</v>
+        <v>44937.57531071849</v>
       </c>
       <c r="B38" t="n">
         <v>181.0437050409912</v>
@@ -1561,7 +1561,7 @@
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>44881.57768443332</v>
+        <v>44937.57739405183</v>
       </c>
       <c r="B39" t="n">
         <v>186.3951912195193</v>
@@ -1590,7 +1590,7 @@
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>44881.57976776666</v>
+        <v>44937.57947738516</v>
       </c>
       <c r="B40" t="n">
         <v>191.2928204493224</v>
@@ -1619,7 +1619,7 @@
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>44881.58185109999</v>
+        <v>44937.58156071849</v>
       </c>
       <c r="B41" t="n">
         <v>195.6779151233904</v>
@@ -1648,7 +1648,7 @@
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>44881.58393443332</v>
+        <v>44937.58364405183</v>
       </c>
       <c r="B42" t="n">
         <v>199.526358868968</v>
@@ -1677,7 +1677,7 @@
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>44881.58601776665</v>
+        <v>44937.58572738517</v>
       </c>
       <c r="B43" t="n">
         <v>202.8391549367546</v>
@@ -1706,7 +1706,7 @@
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>44881.58810109999</v>
+        <v>44937.5878107185</v>
       </c>
       <c r="B44" t="n">
         <v>205.6344288521939</v>
@@ -1735,7 +1735,7 @@
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>44881.59018443332</v>
+        <v>44937.58989405183</v>
       </c>
       <c r="B45" t="n">
         <v>207.9411432007708</v>
@@ -1764,7 +1764,7 @@
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>44881.59226776665</v>
+        <v>44937.59197738516</v>
       </c>
       <c r="B46" t="n">
         <v>209.7944116233752</v>
@@ -1793,7 +1793,7 @@
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>44881.59435109999</v>
+        <v>44937.5940607185</v>
       </c>
       <c r="B47" t="n">
         <v>211.2321533354801</v>
@@ -1822,7 +1822,7 @@
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>44881.59643443332</v>
+        <v>44937.59614405183</v>
       </c>
       <c r="B48" t="n">
         <v>212.2928022449778</v>
@@ -1851,7 +1851,7 @@
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>44881.59851776665</v>
+        <v>44937.59822738516</v>
       </c>
       <c r="B49" t="n">
         <v>213.0138104131109</v>
@@ -1880,7 +1880,7 @@
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
-        <v>44881.60060109999</v>
+        <v>44937.6003107185</v>
       </c>
       <c r="B50" t="n">
         <v>213.4307298855713</v>
@@ -1909,7 +1909,7 @@
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
-        <v>44881.60268443332</v>
+        <v>44937.60239405183</v>
       </c>
       <c r="B51" t="n">
         <v>213.5767032445664</v>
@@ -1938,7 +1938,7 @@
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
-        <v>44881.60476776666</v>
+        <v>44937.60447738516</v>
       </c>
       <c r="B52" t="n">
         <v>213.482234510414</v>
@@ -1967,7 +1967,7 @@
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
-        <v>44881.60685109999</v>
+        <v>44937.60656071849</v>
       </c>
       <c r="B53" t="n">
         <v>213.1751459730963</v>
@@ -1996,7 +1996,7 @@
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
-        <v>44881.60893443332</v>
+        <v>44937.60864405183</v>
       </c>
       <c r="B54" t="n">
         <v>212.6806531424355</v>
@@ -2025,7 +2025,7 @@
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
-        <v>44881.61101776666</v>
+        <v>44937.61072738516</v>
       </c>
       <c r="B55" t="n">
         <v>212.0215101838714</v>
@@ -2054,7 +2054,7 @@
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
-        <v>44881.61310109999</v>
+        <v>44937.61281071849</v>
       </c>
       <c r="B56" t="n">
         <v>211.2181931378731</v>
@@ -2083,7 +2083,7 @@
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
-        <v>44881.61518443332</v>
+        <v>44937.61489405183</v>
       </c>
       <c r="B57" t="n">
         <v>210.2890990511079</v>
@@ -2112,7 +2112,7 @@
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
-        <v>44881.61726776665</v>
+        <v>44937.61697738517</v>
       </c>
       <c r="B58" t="n">
         <v>209.2507468657183</v>
@@ -2141,7 +2141,7 @@
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
-        <v>44881.61935109999</v>
+        <v>44937.6190607185</v>
       </c>
       <c r="B59" t="n">
         <v>208.1179713210128</v>
@@ -2170,7 +2170,7 @@
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
-        <v>44881.62143443332</v>
+        <v>44937.62114405183</v>
       </c>
       <c r="B60" t="n">
         <v>206.9041048443084</v>
@@ -2199,7 +2199,7 @@
     </row>
     <row r="61">
       <c r="A61" s="2" t="n">
-        <v>44881.62351776665</v>
+        <v>44937.62322738516</v>
       </c>
       <c r="B61" t="n">
         <v>205.6211449187058</v>
@@ -2228,7 +2228,7 @@
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
-        <v>44881.62560109999</v>
+        <v>44937.6253107185</v>
       </c>
       <c r="B62" t="n">
         <v>204.2799060680334</v>
@@ -2257,7 +2257,7 @@
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
-        <v>44881.62768443332</v>
+        <v>44937.62739405183</v>
       </c>
       <c r="B63" t="n">
         <v>202.8901566517287</v>
@@ -2286,7 +2286,7 @@
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
-        <v>44881.62976776665</v>
+        <v>44937.62947738516</v>
       </c>
       <c r="B64" t="n">
         <v>201.4607413022461</v>
@@ -2315,7 +2315,7 @@
     </row>
     <row r="65">
       <c r="A65" s="2" t="n">
-        <v>44881.63185109999</v>
+        <v>44937.6315607185</v>
       </c>
       <c r="B65" t="n">
         <v>199.9996901988851</v>
@@ -2344,7 +2344,7 @@
     </row>
     <row r="66">
       <c r="A66" s="2" t="n">
-        <v>44881.63393443332</v>
+        <v>44937.63364405183</v>
       </c>
       <c r="B66" t="n">
         <v>198.5143165499267</v>
@@ -2373,7 +2373,7 @@
     </row>
     <row r="67">
       <c r="A67" s="2" t="n">
-        <v>44881.63601776666</v>
+        <v>44937.63572738516</v>
       </c>
       <c r="B67" t="n">
         <v>197.0113037167519</v>
@@ -2402,7 +2402,7 @@
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
-        <v>44881.63810109999</v>
+        <v>44937.63781071849</v>
       </c>
       <c r="B68" t="n">
         <v>195.4967834061341</v>
@@ -2431,7 +2431,7 @@
     </row>
     <row r="69">
       <c r="A69" s="2" t="n">
-        <v>44881.64018443332</v>
+        <v>44937.63989405183</v>
       </c>
       <c r="B69" t="n">
         <v>193.9764063129518</v>
@@ -2460,7 +2460,7 @@
     </row>
     <row r="70">
       <c r="A70" s="2" t="n">
-        <v>44881.64226776666</v>
+        <v>44937.64197738516</v>
       </c>
       <c r="B70" t="n">
         <v>192.4554065381906</v>
@@ -2489,7 +2489,7 @@
     </row>
     <row r="71">
       <c r="A71" s="2" t="n">
-        <v>44881.64435109999</v>
+        <v>44937.64406071849</v>
       </c>
       <c r="B71" t="n">
         <v>190.9386610528188</v>
@@ -2518,7 +2518,7 @@
     </row>
     <row r="72">
       <c r="A72" s="2" t="n">
-        <v>44881.64643443332</v>
+        <v>44937.64614405183</v>
       </c>
       <c r="B72" t="n">
         <v>189.4307454393996</v>
@@ -2547,7 +2547,7 @@
     </row>
     <row r="73">
       <c r="A73" s="2" t="n">
-        <v>44881.64851776665</v>
+        <v>44937.64822738517</v>
       </c>
       <c r="B73" t="n">
         <v>187.9359871304925</v>
@@ -2576,7 +2576,7 @@
     </row>
     <row r="74">
       <c r="A74" s="2" t="n">
-        <v>44881.65060109999</v>
+        <v>44937.6503107185</v>
       </c>
       <c r="B74" t="n">
         <v>186.4585173857465</v>
@@ -2605,7 +2605,7 @@
     </row>
     <row r="75">
       <c r="A75" s="2" t="n">
-        <v>44881.65268443332</v>
+        <v>44937.65239405183</v>
       </c>
       <c r="B75" t="n">
         <v>185.002323318719</v>
@@ -2634,7 +2634,7 @@
     </row>
     <row r="76">
       <c r="A76" s="2" t="n">
-        <v>44881.65476776665</v>
+        <v>44937.65447738516</v>
       </c>
       <c r="B76" t="n">
         <v>183.5713014127506</v>
@@ -2663,7 +2663,7 @@
     </row>
     <row r="77">
       <c r="A77" s="2" t="n">
-        <v>44881.65685109999</v>
+        <v>44937.6565607185</v>
       </c>
       <c r="B77" t="n">
         <v>182.1692820712786</v>
@@ -2692,7 +2692,7 @@
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
-        <v>44881.65893443332</v>
+        <v>44937.65864405183</v>
       </c>
       <c r="B78" t="n">
         <v>180.7999379120656</v>
@@ -2721,7 +2721,7 @@
     </row>
     <row r="79">
       <c r="A79" s="2" t="n">
-        <v>44881.66101776665</v>
+        <v>44937.66072738516</v>
       </c>
       <c r="B79" t="n">
         <v>179.4822171304289</v>
@@ -2750,7 +2750,7 @@
     </row>
     <row r="80">
       <c r="A80" s="2" t="n">
-        <v>44881.66310109999</v>
+        <v>44937.6628107185</v>
       </c>
       <c r="B80" t="n">
         <v>178.4839860450501</v>
@@ -2779,7 +2779,7 @@
     </row>
     <row r="81">
       <c r="A81" s="2" t="n">
-        <v>44881.66518443332</v>
+        <v>44937.66489405183</v>
       </c>
       <c r="B81" t="n">
         <v>178.2116885846853</v>
@@ -2808,7 +2808,7 @@
     </row>
     <row r="82">
       <c r="A82" s="2" t="n">
-        <v>44881.66726776666</v>
+        <v>44937.66697738516</v>
       </c>
       <c r="B82" t="n">
         <v>178.7758482645653</v>
@@ -2837,7 +2837,7 @@
     </row>
     <row r="83">
       <c r="A83" s="2" t="n">
-        <v>44881.66935109999</v>
+        <v>44937.66906071849</v>
       </c>
       <c r="B83" t="n">
         <v>180.0514351016218</v>
@@ -2866,7 +2866,7 @@
     </row>
     <row r="84">
       <c r="A84" s="2" t="n">
-        <v>44881.67143443332</v>
+        <v>44937.67114405183</v>
       </c>
       <c r="B84" t="n">
         <v>181.7944394676312</v>
@@ -2895,7 +2895,7 @@
     </row>
     <row r="85">
       <c r="A85" s="2" t="n">
-        <v>44881.67351776666</v>
+        <v>44937.67322738516</v>
       </c>
       <c r="B85" t="n">
         <v>183.7412763872546</v>
@@ -2924,7 +2924,7 @@
     </row>
     <row r="86">
       <c r="A86" s="2" t="n">
-        <v>44881.67560109999</v>
+        <v>44937.67531071849</v>
       </c>
       <c r="B86" t="n">
         <v>185.6697358658026</v>
@@ -2953,7 +2953,7 @@
     </row>
     <row r="87">
       <c r="A87" s="2" t="n">
-        <v>44881.67768443332</v>
+        <v>44937.67739405183</v>
       </c>
       <c r="B87" t="n">
         <v>187.4195266421568</v>
@@ -2982,7 +2982,7 @@
     </row>
     <row r="88">
       <c r="A88" s="2" t="n">
-        <v>44881.67976776665</v>
+        <v>44937.67947738517</v>
       </c>
       <c r="B88" t="n">
         <v>188.8893523885694</v>
@@ -3011,7 +3011,7 @@
     </row>
     <row r="89">
       <c r="A89" s="2" t="n">
-        <v>44881.68185109999</v>
+        <v>44937.6815607185</v>
       </c>
       <c r="B89" t="n">
         <v>190.0252116248384</v>
@@ -3040,7 +3040,7 @@
     </row>
     <row r="90">
       <c r="A90" s="2" t="n">
-        <v>44881.68393443332</v>
+        <v>44937.68364405183</v>
       </c>
       <c r="B90" t="n">
         <v>190.8074936707712</v>
@@ -3069,7 +3069,7 @@
     </row>
     <row r="91">
       <c r="A91" s="2" t="n">
-        <v>44881.68601776665</v>
+        <v>44937.68572738516</v>
       </c>
       <c r="B91" t="n">
         <v>191.2398290098539</v>
@@ -3098,7 +3098,7 @@
     </row>
     <row r="92">
       <c r="A92" s="2" t="n">
-        <v>44881.68810109999</v>
+        <v>44937.6878107185</v>
       </c>
       <c r="B92" t="n">
         <v>191.3404472119197</v>
@@ -3127,7 +3127,7 @@
     </row>
     <row r="93">
       <c r="A93" s="2" t="n">
-        <v>44881.69018443332</v>
+        <v>44937.68989405183</v>
       </c>
       <c r="B93" t="n">
         <v>191.1358996246695</v>
@@ -3156,7 +3156,7 @@
     </row>
     <row r="94">
       <c r="A94" s="2" t="n">
-        <v>44881.69226776665</v>
+        <v>44937.69197738516</v>
       </c>
       <c r="B94" t="n">
         <v>190.6567151396728</v>
@@ -3185,7 +3185,7 @@
     </row>
     <row r="95">
       <c r="A95" s="2" t="n">
-        <v>44881.69435109999</v>
+        <v>44937.6940607185</v>
       </c>
       <c r="B95" t="n">
         <v>189.934524240508</v>
@@ -3214,7 +3214,7 @@
     </row>
     <row r="96">
       <c r="A96" s="2" t="n">
-        <v>44881.69643443332</v>
+        <v>44937.69614405183</v>
       </c>
       <c r="B96" t="n">
         <v>189.0002474406641</v>
@@ -3243,7 +3243,7 @@
     </row>
     <row r="97">
       <c r="A97" s="2" t="n">
-        <v>44881.69851776666</v>
+        <v>44937.69822738516</v>
       </c>
       <c r="B97" t="n">
         <v>187.8830287097096</v>
@@ -3272,7 +3272,7 @@
     </row>
     <row r="98">
       <c r="A98" s="2" t="n">
-        <v>44881.70060109999</v>
+        <v>44937.70031071849</v>
       </c>
       <c r="B98" t="n">
         <v>186.6096744444968</v>
@@ -3301,7 +3301,7 @@
     </row>
     <row r="99">
       <c r="A99" s="2" t="n">
-        <v>44881.70268443332</v>
+        <v>44937.70239405183</v>
       </c>
       <c r="B99" t="n">
         <v>185.204424748465</v>
@@ -3330,7 +3330,7 @@
     </row>
     <row r="100">
       <c r="A100" s="2" t="n">
-        <v>44881.70476776666</v>
+        <v>44937.70447738516</v>
       </c>
       <c r="B100" t="n">
         <v>183.6889329721793</v>
@@ -3359,7 +3359,7 @@
     </row>
     <row r="101">
       <c r="A101" s="2" t="n">
-        <v>44881.70685109999</v>
+        <v>44937.70656071849</v>
       </c>
       <c r="B101" t="n">
         <v>182.0822422365885</v>
@@ -3388,7 +3388,7 @@
     </row>
     <row r="102">
       <c r="A102" s="2" t="n">
-        <v>44881.70893443332</v>
+        <v>44937.70864405183</v>
       </c>
       <c r="B102" t="n">
         <v>180.4008097349049</v>
@@ -3417,7 +3417,7 @@
     </row>
     <row r="103">
       <c r="A103" s="2" t="n">
-        <v>44881.71101776665</v>
+        <v>44937.71072738517</v>
       </c>
       <c r="B103" t="n">
         <v>178.6590636911429</v>
@@ -3446,7 +3446,7 @@
     </row>
     <row r="104">
       <c r="A104" s="2" t="n">
-        <v>44881.71310109999</v>
+        <v>44937.7128107185</v>
       </c>
       <c r="B104" t="n">
         <v>176.8696886194843</v>
@@ -3475,7 +3475,7 @@
     </row>
     <row r="105">
       <c r="A105" s="2" t="n">
-        <v>44881.71518443332</v>
+        <v>44937.71489405183</v>
       </c>
       <c r="B105" t="n">
         <v>175.0438008299371</v>
@@ -3504,7 +3504,7 @@
     </row>
     <row r="106">
       <c r="A106" s="2" t="n">
-        <v>44881.71726776665</v>
+        <v>44937.71697738516</v>
       </c>
       <c r="B106" t="n">
         <v>173.1911237361004</v>
@@ -3533,7 +3533,7 @@
     </row>
     <row r="107">
       <c r="A107" s="2" t="n">
-        <v>44881.71935109999</v>
+        <v>44937.7190607185</v>
       </c>
       <c r="B107" t="n">
         <v>171.3201546577692</v>
@@ -3562,7 +3562,7 @@
     </row>
     <row r="108">
       <c r="A108" s="2" t="n">
-        <v>44881.72143443332</v>
+        <v>44937.72114405183</v>
       </c>
       <c r="B108" t="n">
         <v>169.4754007311149</v>
@@ -3591,7 +3591,7 @@
     </row>
     <row r="109">
       <c r="A109" s="2" t="n">
-        <v>44881.72351776665</v>
+        <v>44937.72322738516</v>
       </c>
       <c r="B109" t="n">
         <v>167.9109462790697</v>
@@ -3620,7 +3620,7 @@
     </row>
     <row r="110">
       <c r="A110" s="2" t="n">
-        <v>44881.72560109999</v>
+        <v>44937.7253107185</v>
       </c>
       <c r="B110" t="n">
         <v>166.8699132621484</v>
@@ -3649,7 +3649,7 @@
     </row>
     <row r="111">
       <c r="A111" s="2" t="n">
-        <v>44881.72768443332</v>
+        <v>44937.72739405183</v>
       </c>
       <c r="B111" t="n">
         <v>166.4622377596964</v>
@@ -3678,7 +3678,7 @@
     </row>
     <row r="112">
       <c r="A112" s="2" t="n">
-        <v>44881.72976776666</v>
+        <v>44937.72947738516</v>
       </c>
       <c r="B112" t="n">
         <v>166.7463068947553</v>
@@ -3707,7 +3707,7 @@
     </row>
     <row r="113">
       <c r="A113" s="2" t="n">
-        <v>44881.73185109999</v>
+        <v>44937.73156071849</v>
       </c>
       <c r="B113" t="n">
         <v>167.7722512678529</v>
@@ -3736,7 +3736,7 @@
     </row>
     <row r="114">
       <c r="A114" s="2" t="n">
-        <v>44881.73393443332</v>
+        <v>44937.73364405183</v>
       </c>
       <c r="B114" t="n">
         <v>169.5892184828768</v>
@@ -3765,7 +3765,7 @@
     </row>
     <row r="115">
       <c r="A115" s="2" t="n">
-        <v>44881.73601776666</v>
+        <v>44937.73572738516</v>
       </c>
       <c r="B115" t="n">
         <v>172.1916501642761</v>
@@ -3794,7 +3794,7 @@
     </row>
     <row r="116">
       <c r="A116" s="2" t="n">
-        <v>44881.73810109999</v>
+        <v>44937.73781071849</v>
       </c>
       <c r="B116" t="n">
         <v>175.4810192208173</v>
@@ -3823,7 +3823,7 @@
     </row>
     <row r="117">
       <c r="A117" s="2" t="n">
-        <v>44881.74018443332</v>
+        <v>44937.73989405183</v>
       </c>
       <c r="B117" t="n">
         <v>179.2735499924243</v>
@@ -3852,7 +3852,7 @@
     </row>
     <row r="118">
       <c r="A118" s="2" t="n">
-        <v>44881.74226776665</v>
+        <v>44937.74197738517</v>
       </c>
       <c r="B118" t="n">
         <v>183.3361284704601</v>
@@ -3881,7 +3881,7 @@
     </row>
     <row r="119">
       <c r="A119" s="2" t="n">
-        <v>44881.74435109999</v>
+        <v>44937.7440607185</v>
       </c>
       <c r="B119" t="n">
         <v>187.4316183747051</v>
@@ -3910,7 +3910,7 @@
     </row>
     <row r="120">
       <c r="A120" s="2" t="n">
-        <v>44881.74643443332</v>
+        <v>44937.74614405183</v>
       </c>
       <c r="B120" t="n">
         <v>191.3535905976206</v>
@@ -3939,7 +3939,7 @@
     </row>
     <row r="121">
       <c r="A121" s="2" t="n">
-        <v>44881.74851776665</v>
+        <v>44937.74822738516</v>
       </c>
       <c r="B121" t="n">
         <v>194.9432319349993</v>
@@ -3968,7 +3968,7 @@
     </row>
     <row r="122">
       <c r="A122" s="2" t="n">
-        <v>44881.75060109999</v>
+        <v>44937.7503107185</v>
       </c>
       <c r="B122" t="n">
         <v>198.0918901444067</v>

</xml_diff>